<commit_message>
individual data sets contained date-time-objects
</commit_message>
<xml_diff>
--- a/Projects/merinehlsen/flydata.xlsx
+++ b/Projects/merinehlsen/flydata.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merinehlsen/Desktop/R2_DataProjects/R2_Data_Projects_Git/Projects/merinehlsen/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan-t\OneDrive - bwedu\Studium\Modul 09 Wahlpflicht\Github and R\Data-projects-with-R-and-GitHub\Projects\merinehlsen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CC9C09-58EE-AC4C-AF0C-6D0E2B502EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE67B07B-0F3A-4ADB-9764-18F13344E89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="1240" windowWidth="27840" windowHeight="16660" xr2:uid="{D33EACD9-9642-4541-B947-3DD8A3B2FF67}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{D33EACD9-9642-4541-B947-3DD8A3B2FF67}"/>
   </bookViews>
   <sheets>
-    <sheet name="Survival" sheetId="1" r:id="rId1"/>
+    <sheet name="Survival" sheetId="4" r:id="rId1"/>
     <sheet name="Developmental_Time" sheetId="2" r:id="rId2"/>
     <sheet name="Metabolic_Pools" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -119,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -139,6 +139,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,16 +164,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{F0D52011-DE42-45D5-9E0D-27556A672032}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -182,7 +193,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -497,569 +508,572 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94976CE6-E5A6-E842-B41D-46C3C567CFE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C847FC8B-D073-489B-9BD6-F5C213F50327}">
   <dimension ref="A1:AE69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="16384" width="10.6640625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:31">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>3</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>4</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <v>5</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="2">
         <v>2</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="2">
         <v>3</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="2">
         <v>4</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="2">
         <v>5</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="2">
         <v>1</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="2">
         <v>2</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="2">
         <v>3</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="2">
         <v>4</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:31">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="B3" s="3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
-        <v>10</v>
-      </c>
-      <c r="H3" s="1">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="F3" s="3">
+        <v>10</v>
+      </c>
+      <c r="H3" s="3">
+        <v>10</v>
+      </c>
+      <c r="J3" s="3">
         <v>7</v>
       </c>
-      <c r="L3" s="1">
-        <v>10</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="L3" s="3">
+        <v>10</v>
+      </c>
+      <c r="N3" s="3">
         <v>5</v>
       </c>
-      <c r="P3" s="1">
-        <v>10</v>
-      </c>
-      <c r="R3" s="1">
-        <v>10</v>
-      </c>
-      <c r="T3" s="1">
+      <c r="P3" s="3">
+        <v>10</v>
+      </c>
+      <c r="R3" s="3">
+        <v>10</v>
+      </c>
+      <c r="T3" s="3">
         <v>6</v>
       </c>
-      <c r="V3" s="1">
-        <v>10</v>
-      </c>
-      <c r="X3" s="1">
+      <c r="V3" s="3">
+        <v>10</v>
+      </c>
+      <c r="X3" s="3">
         <v>5</v>
       </c>
-      <c r="Z3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>10</v>
-      </c>
-      <c r="AD3" s="1">
+      <c r="Z3" s="3">
+        <v>10</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>10</v>
+      </c>
+      <c r="AD3" s="3">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:31">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>17.8</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.1399999999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>13.4</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>1.03</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>1.02</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>15.5</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>1.63</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>18.3</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
         <v>1.71</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="2">
         <v>19</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <v>1.26</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <v>1.63</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <v>19.899999999999999</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="2">
         <v>1.23</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="2">
         <v>14.7</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="2">
         <v>0.9</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="2">
         <v>18.8</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="2">
         <v>1.3</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="2">
         <v>16.899999999999999</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="2">
         <v>1.37</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="2">
         <v>16.2</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="2">
         <v>1.1100000000000001</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="2">
         <v>18.5</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="2">
         <v>0.93</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="2">
         <v>19.399999999999999</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="2">
         <v>0.82</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="2">
         <v>18.100000000000001</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="2">
         <v>1.39</v>
       </c>
     </row>
     <row r="5" spans="1:31">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>17.8</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.57299999999999995</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>16.8</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>1.2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>1.29</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>13.7</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>1.1599999999999999</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <v>15.6</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="2">
         <v>1.76</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="2">
         <v>18</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="2">
         <v>0.77</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="2">
         <v>11</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="2">
         <v>1.82</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="2">
         <v>14.9</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="2">
         <v>1.57</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="2">
         <v>15.3</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="2">
         <v>1.1200000000000001</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="2">
         <v>13.2</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="2">
         <v>1.3</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="2">
         <v>16.2</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="2">
         <v>0.92</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="2">
         <v>18.399999999999999</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="2">
         <v>0.93</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="2">
         <v>0.8</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="2">
         <v>14</v>
       </c>
-      <c r="AC5">
+      <c r="AC5" s="2">
         <v>0.77</v>
       </c>
-      <c r="AD5">
+      <c r="AD5" s="2">
         <v>15</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="2">
         <v>1.36</v>
       </c>
     </row>
     <row r="6" spans="1:31">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>35.6</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.78</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>30.2</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>1.07</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>32.200000000000003</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>0.83</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>29.2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>1.2</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
         <v>33.9</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="2">
         <v>1.3</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="2">
         <v>37</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="2">
         <v>1.17</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="2">
         <v>27.4</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="2">
         <v>2.62</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="2">
         <v>34.799999999999997</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="2">
         <v>1.45</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="2">
         <v>30</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="2">
         <v>1.32</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="2">
         <v>32</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="2">
         <v>1.03</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="2">
         <v>33.1</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="2">
         <v>1.39</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="2">
         <v>34.6</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="2">
         <v>1.4</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="2">
         <v>34.6</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="2">
         <v>0.65</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="2">
         <v>33.4</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" s="2">
         <v>0.96</v>
       </c>
-      <c r="AD6">
+      <c r="AD6" s="2">
         <v>33.1</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="2">
         <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:31">
-      <c r="A8" s="2"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="10" spans="1:31">
-      <c r="A10" s="1"/>
+      <c r="A10" s="3"/>
     </row>
     <row r="11" spans="1:31">
-      <c r="A11" s="1"/>
+      <c r="A11" s="3"/>
     </row>
     <row r="12" spans="1:31">
-      <c r="A12" s="1"/>
+      <c r="A12" s="3"/>
     </row>
     <row r="13" spans="1:31">
-      <c r="A13" s="1"/>
+      <c r="A13" s="3"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="1"/>
+      <c r="A18" s="3"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="1"/>
+      <c r="A19" s="3"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="1"/>
+      <c r="A20" s="3"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="1"/>
+      <c r="A21" s="3"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="1"/>
+      <c r="A22" s="3"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="1"/>
+      <c r="A23" s="3"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="1"/>
+      <c r="A24" s="3"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="1"/>
+      <c r="A26" s="3"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="1"/>
+      <c r="A27" s="3"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="1"/>
+      <c r="A28" s="3"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="1"/>
+      <c r="A29" s="3"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="1"/>
+      <c r="A30" s="3"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="1"/>
+      <c r="A31" s="3"/>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="1"/>
+      <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="1"/>
+      <c r="A33" s="3"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="1"/>
+      <c r="A41" s="3"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="1"/>
+      <c r="A43" s="3"/>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="1"/>
+      <c r="A45" s="3"/>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="1"/>
+      <c r="A47" s="3"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="1"/>
+      <c r="A49" s="3"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="1"/>
+      <c r="A51" s="3"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="1"/>
+      <c r="A53" s="3"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="1"/>
+      <c r="A55" s="3"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="1"/>
+      <c r="A57" s="3"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="1"/>
+      <c r="A58" s="3"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="1"/>
+      <c r="A59" s="3"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="1"/>
+      <c r="A60" s="3"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="1"/>
+      <c r="A61" s="3"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="1"/>
+      <c r="A62" s="3"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="1"/>
+      <c r="A63" s="3"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="1"/>
+      <c r="A64" s="3"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="1"/>
+      <c r="A65" s="3"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="1"/>
+      <c r="A67" s="3"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="1"/>
+      <c r="A68" s="3"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="1"/>
+      <c r="A69" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1071,11 +1085,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{883FD7D9-EA1D-3D48-ACBE-A4EF8A948944}">
   <dimension ref="A1:AE6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
@@ -1522,10 +1536,10 @@
   <dimension ref="A1:U58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" t="s">

</xml_diff>